<commit_message>
Rawdata KW6+7 & preliminary analysis
</commit_message>
<xml_diff>
--- a/Data/Prep data/20201123_Sample number estimation.xlsx
+++ b/Data/Prep data/20201123_Sample number estimation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ursel\Google Drive\Post-doc Spain\Part II_Barcelona\Workshops and Questionnaire\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ursel\Google Drive\Post-doc Spain\Part II_Barcelona\Questionnaires\Data\Prep data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB0FFD82-A544-41B1-A0A5-819CE7B4D527}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC0522FA-9786-4FAD-93EC-53D7CCB2AB57}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" firstSheet="4" activeTab="6" xr2:uid="{B5CD7DA6-057F-4DB6-9E4B-BDE59985C93A}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="6" xr2:uid="{B5CD7DA6-057F-4DB6-9E4B-BDE59985C93A}"/>
   </bookViews>
   <sheets>
     <sheet name="Landings per group per fleet" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,8 @@
     <sheet name="Relative group composition (2)" sheetId="7" r:id="rId5"/>
     <sheet name="List of species for question" sheetId="4" r:id="rId6"/>
     <sheet name="Tabelle5" sheetId="5" r:id="rId7"/>
+    <sheet name="Tabelle1" sheetId="8" r:id="rId8"/>
+    <sheet name="Tabelle2" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1505" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1855" uniqueCount="273">
   <si>
     <t>Group name</t>
   </si>
@@ -772,6 +774,93 @@
   </si>
   <si>
     <t>Squid</t>
+  </si>
+  <si>
+    <t>Lethrinus_harak</t>
+  </si>
+  <si>
+    <t>Lethrinus_variegatus</t>
+  </si>
+  <si>
+    <t>Lethrinus_mahsena</t>
+  </si>
+  <si>
+    <t>Plecthorinchus_gibbus</t>
+  </si>
+  <si>
+    <t>FootFisher</t>
+  </si>
+  <si>
+    <t>Group_name</t>
+  </si>
+  <si>
+    <t>Siganus_sutor</t>
+  </si>
+  <si>
+    <t>Leptoscarus_vaigiensis</t>
+  </si>
+  <si>
+    <t>Lethrinus_lentjan</t>
+  </si>
+  <si>
+    <t>Lethrinus_borbonicus</t>
+  </si>
+  <si>
+    <t>Lutjanus_fulviflamma</t>
+  </si>
+  <si>
+    <t>Scarus_ghobban</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Snails</t>
+  </si>
+  <si>
+    <t>Sardinella_spp</t>
+  </si>
+  <si>
+    <t>Siganus_stellatus</t>
+  </si>
+  <si>
+    <t>Calatomus_carolinus</t>
+  </si>
+  <si>
+    <t>Hipposcarus_harid</t>
+  </si>
+  <si>
+    <t>Monodactylus_argenteus</t>
+  </si>
+  <si>
+    <t>Cheilinus_trilobatus</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Species</t>
+  </si>
+  <si>
+    <t>Plectorhinchus_gibbus</t>
+  </si>
+  <si>
+    <t>Balistidae</t>
+  </si>
+  <si>
+    <t>Mugilidae</t>
+  </si>
+  <si>
+    <t>Monodactylus_argentus</t>
+  </si>
+  <si>
+    <t>Acanthurus_spp</t>
+  </si>
+  <si>
+    <t>Caesionidae</t>
+  </si>
+  <si>
+    <t>Crabs_Lobsters</t>
   </si>
 </sst>
 </file>
@@ -832,7 +921,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -846,6 +935,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
@@ -1175,7 +1267,7 @@
   <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B2" sqref="B2:L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1299,7 +1391,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>252</v>
       </c>
       <c r="C4">
         <v>5.4845409999999997E-2</v>
@@ -1337,7 +1429,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>253</v>
       </c>
       <c r="C5">
         <v>4.0705789999999999E-2</v>
@@ -1375,7 +1467,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>254</v>
       </c>
       <c r="C6">
         <v>5.85841E-2</v>
@@ -1413,7 +1505,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>255</v>
       </c>
       <c r="C7">
         <v>1.7590459999999999E-2</v>
@@ -2330,18 +2422,18 @@
   <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="2" max="2" width="21.76953125" customWidth="1"/>
+    <col min="2" max="2" width="24.6328125" customWidth="1"/>
     <col min="3" max="3" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.75">
       <c r="B1" t="s">
-        <v>0</v>
+        <v>249</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -2368,7 +2460,7 @@
         <v>8</v>
       </c>
       <c r="K1" t="s">
-        <v>9</v>
+        <v>248</v>
       </c>
       <c r="L1" t="s">
         <v>10</v>
@@ -2379,7 +2471,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>250</v>
       </c>
       <c r="C2" s="4">
         <f>'Landings per group per fleet'!C2/'Landings per group per fleet'!C$30</f>
@@ -2426,7 +2518,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>251</v>
       </c>
       <c r="C3" s="4">
         <f>'Landings per group per fleet'!C3/'Landings per group per fleet'!C$30</f>
@@ -2473,7 +2565,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>252</v>
       </c>
       <c r="C4" s="4">
         <f>'Landings per group per fleet'!C4/'Landings per group per fleet'!C$30</f>
@@ -2520,7 +2612,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>253</v>
       </c>
       <c r="C5" s="4">
         <f>'Landings per group per fleet'!C5/'Landings per group per fleet'!C$30</f>
@@ -2567,7 +2659,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>254</v>
       </c>
       <c r="C6" s="4">
         <f>'Landings per group per fleet'!C6/'Landings per group per fleet'!C$30</f>
@@ -2614,7 +2706,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>255</v>
       </c>
       <c r="C7" s="4">
         <f>'Landings per group per fleet'!C7/'Landings per group per fleet'!C$30</f>
@@ -3746,12 +3838,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE104033-CFBA-43C2-98B6-1A931D52390E}">
   <dimension ref="A1:R79"/>
   <sheetViews>
-    <sheetView topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A78"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="M82" sqref="M82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
+    <col min="2" max="2" width="17.58984375" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="6" max="6" width="7.6796875" customWidth="1"/>
     <col min="7" max="15" width="4.1796875" customWidth="1"/>
@@ -7561,7 +7654,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5E79516-93D0-4C9E-84B3-DB569B02CE9E}">
   <dimension ref="A1:Q80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="A79" sqref="A2:A79"/>
     </sheetView>
   </sheetViews>
@@ -11526,7 +11619,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21FD7DFE-547D-409D-8698-691D77B246AC}">
   <dimension ref="A1:P80"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
@@ -16271,7 +16364,7 @@
   <dimension ref="A1:P27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="O2" sqref="O2:O27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -17616,8 +17709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19F8B279-3A6A-4B64-B7AD-F14FF1FD7816}">
   <dimension ref="A1:P46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C34" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36:D45"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -18680,12 +18773,10 @@
         <v>10</v>
       </c>
       <c r="J29">
-        <f>J24</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K29">
-        <f>K27</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L29">
         <f>L27</f>
@@ -18705,7 +18796,7 @@
       </c>
       <c r="P29" s="10">
         <f>SUM(F29:O29)</f>
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="36" spans="3:4" x14ac:dyDescent="0.75">
@@ -18802,4 +18893,3499 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE5E229B-79FC-44A1-A567-767FE675A598}">
+  <dimension ref="A1:O33"/>
+  <sheetViews>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7:O33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="2" max="5" width="26.7265625" customWidth="1"/>
+    <col min="6" max="6" width="25.36328125" customWidth="1"/>
+    <col min="7" max="15" width="12.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A1" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" t="s">
+        <v>248</v>
+      </c>
+      <c r="O1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B2" t="s">
+        <v>250</v>
+      </c>
+      <c r="C2" t="s">
+        <v>213</v>
+      </c>
+      <c r="D2" t="s">
+        <v>250</v>
+      </c>
+      <c r="E2" t="s">
+        <v>250</v>
+      </c>
+      <c r="F2" s="13">
+        <v>0.24327516632290566</v>
+      </c>
+      <c r="G2" s="13">
+        <v>2.6887481193671684E-3</v>
+      </c>
+      <c r="H2" s="13">
+        <v>0.33493190218392843</v>
+      </c>
+      <c r="I2" s="13">
+        <v>5.1120010312894412E-2</v>
+      </c>
+      <c r="J2" s="13">
+        <v>3.9191572632297188E-2</v>
+      </c>
+      <c r="K2" s="13">
+        <v>0</v>
+      </c>
+      <c r="L2" s="13">
+        <v>0</v>
+      </c>
+      <c r="M2" s="13">
+        <v>0</v>
+      </c>
+      <c r="N2" s="13">
+        <v>0</v>
+      </c>
+      <c r="O2" s="13">
+        <f>SUM(F2:N2)</f>
+        <v>0.67120739957139286</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A3" t="s">
+        <v>223</v>
+      </c>
+      <c r="B3" t="s">
+        <v>251</v>
+      </c>
+      <c r="C3" t="s">
+        <v>192</v>
+      </c>
+      <c r="D3" t="s">
+        <v>251</v>
+      </c>
+      <c r="E3" t="s">
+        <v>251</v>
+      </c>
+      <c r="F3" s="13">
+        <v>5.5753970181862074E-2</v>
+      </c>
+      <c r="G3" s="13">
+        <v>0</v>
+      </c>
+      <c r="H3" s="13">
+        <v>6.9424436980399934E-2</v>
+      </c>
+      <c r="I3" s="13">
+        <v>3.2870947916885267E-2</v>
+      </c>
+      <c r="J3" s="13">
+        <v>1.6535176793197341E-4</v>
+      </c>
+      <c r="K3" s="13">
+        <v>0</v>
+      </c>
+      <c r="L3" s="13">
+        <v>0</v>
+      </c>
+      <c r="M3" s="13">
+        <v>0</v>
+      </c>
+      <c r="N3" s="13">
+        <v>0</v>
+      </c>
+      <c r="O3" s="13">
+        <f t="shared" ref="O3:O33" si="0">SUM(F3:N3)</f>
+        <v>0.15821470684707925</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A4" t="s">
+        <v>224</v>
+      </c>
+      <c r="B4" t="s">
+        <v>252</v>
+      </c>
+      <c r="C4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4" t="s">
+        <v>252</v>
+      </c>
+      <c r="E4" t="s">
+        <v>252</v>
+      </c>
+      <c r="F4" s="13">
+        <v>4.037197589698064E-2</v>
+      </c>
+      <c r="G4" s="13">
+        <v>1.8200770942121311E-4</v>
+      </c>
+      <c r="H4" s="13">
+        <v>7.0103328917493338E-2</v>
+      </c>
+      <c r="I4" s="13">
+        <v>1.6498640436739088E-2</v>
+      </c>
+      <c r="J4" s="13">
+        <v>4.3974169783264995E-2</v>
+      </c>
+      <c r="K4" s="13">
+        <v>0</v>
+      </c>
+      <c r="L4" s="13">
+        <v>2.1945788028398454E-3</v>
+      </c>
+      <c r="M4" s="13">
+        <v>0</v>
+      </c>
+      <c r="N4" s="13">
+        <v>0</v>
+      </c>
+      <c r="O4" s="13">
+        <f t="shared" si="0"/>
+        <v>0.17332470154673912</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A5" t="s">
+        <v>226</v>
+      </c>
+      <c r="B5" t="s">
+        <v>253</v>
+      </c>
+      <c r="C5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" t="s">
+        <v>253</v>
+      </c>
+      <c r="E5" t="s">
+        <v>253</v>
+      </c>
+      <c r="F5" s="13">
+        <v>2.9963732110810288E-2</v>
+      </c>
+      <c r="G5" s="13">
+        <v>6.4529920729672742E-4</v>
+      </c>
+      <c r="H5" s="13">
+        <v>1.934132704684615E-2</v>
+      </c>
+      <c r="I5" s="13">
+        <v>5.2004472918159381E-3</v>
+      </c>
+      <c r="J5" s="13">
+        <v>0.13104542294545901</v>
+      </c>
+      <c r="K5" s="13">
+        <v>0</v>
+      </c>
+      <c r="L5" s="13">
+        <v>0</v>
+      </c>
+      <c r="M5" s="13">
+        <v>0</v>
+      </c>
+      <c r="N5" s="13">
+        <v>0</v>
+      </c>
+      <c r="O5" s="13">
+        <f t="shared" si="0"/>
+        <v>0.18619622860222812</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A6" t="s">
+        <v>227</v>
+      </c>
+      <c r="B6" t="s">
+        <v>254</v>
+      </c>
+      <c r="C6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D6" t="s">
+        <v>254</v>
+      </c>
+      <c r="E6" t="s">
+        <v>254</v>
+      </c>
+      <c r="F6" s="13">
+        <v>4.3124043983740909E-2</v>
+      </c>
+      <c r="G6" s="13">
+        <v>3.1023977375229663E-4</v>
+      </c>
+      <c r="H6" s="13">
+        <v>1.9645168132238763E-2</v>
+      </c>
+      <c r="I6" s="13">
+        <v>2.6214873951847179E-3</v>
+      </c>
+      <c r="J6" s="13">
+        <v>4.011703738630585E-2</v>
+      </c>
+      <c r="K6" s="13">
+        <v>0</v>
+      </c>
+      <c r="L6" s="13">
+        <v>0</v>
+      </c>
+      <c r="M6" s="13">
+        <v>0</v>
+      </c>
+      <c r="N6" s="13">
+        <v>0</v>
+      </c>
+      <c r="O6" s="13">
+        <f t="shared" si="0"/>
+        <v>0.10581797667122253</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A7" t="s">
+        <v>225</v>
+      </c>
+      <c r="B7" t="s">
+        <v>255</v>
+      </c>
+      <c r="C7" t="s">
+        <v>192</v>
+      </c>
+      <c r="D7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E7" t="s">
+        <v>255</v>
+      </c>
+      <c r="F7" s="13">
+        <v>1.2948424072986273E-2</v>
+      </c>
+      <c r="G7" s="13">
+        <v>0</v>
+      </c>
+      <c r="H7" s="13">
+        <v>8.5913053153500854E-2</v>
+      </c>
+      <c r="I7" s="13">
+        <v>4.4007015166550242E-2</v>
+      </c>
+      <c r="J7" s="13">
+        <v>1.5762981892617364E-2</v>
+      </c>
+      <c r="K7" s="13">
+        <v>0</v>
+      </c>
+      <c r="L7" s="13">
+        <v>0</v>
+      </c>
+      <c r="M7" s="13">
+        <v>0</v>
+      </c>
+      <c r="N7" s="13">
+        <v>0</v>
+      </c>
+      <c r="O7" s="13">
+        <f t="shared" si="0"/>
+        <v>0.15863147428565472</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A8" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" s="13">
+        <v>2.8835537410783922E-2</v>
+      </c>
+      <c r="G8" s="13">
+        <v>0.56301632021029757</v>
+      </c>
+      <c r="H8" s="13">
+        <v>2.3000576588516522E-2</v>
+      </c>
+      <c r="I8" s="13">
+        <v>1.2170417835426085E-3</v>
+      </c>
+      <c r="J8" s="13">
+        <v>5.3827866278242625E-2</v>
+      </c>
+      <c r="K8" s="13">
+        <v>0</v>
+      </c>
+      <c r="L8" s="13">
+        <v>0</v>
+      </c>
+      <c r="M8" s="13">
+        <v>0.74414206726848187</v>
+      </c>
+      <c r="N8" s="13">
+        <v>0</v>
+      </c>
+      <c r="O8" s="13">
+        <f t="shared" si="0"/>
+        <v>1.4140394095398652</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A9" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="F9" s="13">
+        <v>8.5052588210217966E-2</v>
+      </c>
+      <c r="G9" s="13">
+        <v>5.0572808725185277E-2</v>
+      </c>
+      <c r="H9" s="13">
+        <v>7.2136199884180723E-3</v>
+      </c>
+      <c r="I9" s="13">
+        <v>0</v>
+      </c>
+      <c r="J9" s="13">
+        <v>1.5842104495929988E-4</v>
+      </c>
+      <c r="K9" s="13">
+        <v>0</v>
+      </c>
+      <c r="L9" s="13">
+        <v>0</v>
+      </c>
+      <c r="M9" s="13">
+        <v>4.5530375519862033E-2</v>
+      </c>
+      <c r="N9" s="13">
+        <v>0</v>
+      </c>
+      <c r="O9" s="13">
+        <f t="shared" si="0"/>
+        <v>0.18852781348864264</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A10" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="F10" s="13">
+        <v>0.17314090764383588</v>
+      </c>
+      <c r="G10" s="13">
+        <v>3.7164125160699127E-2</v>
+      </c>
+      <c r="H10" s="13">
+        <v>0.11619068425536462</v>
+      </c>
+      <c r="I10" s="13">
+        <v>0</v>
+      </c>
+      <c r="J10" s="13">
+        <v>5.3955707526912068E-3</v>
+      </c>
+      <c r="K10" s="13">
+        <v>0</v>
+      </c>
+      <c r="L10" s="13">
+        <v>5.8202799201663982E-3</v>
+      </c>
+      <c r="M10" s="13">
+        <v>0</v>
+      </c>
+      <c r="N10" s="13">
+        <v>0</v>
+      </c>
+      <c r="O10" s="13">
+        <f t="shared" si="0"/>
+        <v>0.33771156773275718</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A11" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>244</v>
+      </c>
+      <c r="F11" s="13">
+        <v>0.19076023000471143</v>
+      </c>
+      <c r="G11" s="13">
+        <v>0</v>
+      </c>
+      <c r="H11" s="13">
+        <v>4.5816576173166521E-2</v>
+      </c>
+      <c r="I11" s="13">
+        <v>6.1008847479864488E-3</v>
+      </c>
+      <c r="J11" s="13">
+        <v>1.1028052915797032E-2</v>
+      </c>
+      <c r="K11" s="13">
+        <v>0</v>
+      </c>
+      <c r="L11" s="13">
+        <v>0</v>
+      </c>
+      <c r="M11" s="13">
+        <v>1.1502410657649354E-2</v>
+      </c>
+      <c r="N11" s="13">
+        <v>1.0693183219853868E-2</v>
+      </c>
+      <c r="O11" s="13">
+        <f t="shared" si="0"/>
+        <v>0.27590133771916464</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A12" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>245</v>
+      </c>
+      <c r="F12" s="13">
+        <v>2.862252193928147E-3</v>
+      </c>
+      <c r="G12" s="13">
+        <v>0</v>
+      </c>
+      <c r="H12" s="13">
+        <v>6.9797803814194382E-3</v>
+      </c>
+      <c r="I12" s="13">
+        <v>4.7180526158804399E-3</v>
+      </c>
+      <c r="J12" s="13">
+        <v>8.3331028170990654E-2</v>
+      </c>
+      <c r="K12" s="13">
+        <v>0</v>
+      </c>
+      <c r="L12" s="13">
+        <v>4.7927583169298911E-2</v>
+      </c>
+      <c r="M12" s="13">
+        <v>0</v>
+      </c>
+      <c r="N12" s="13">
+        <v>0</v>
+      </c>
+      <c r="O12" s="13">
+        <f t="shared" si="0"/>
+        <v>0.14581869653151758</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A13" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>246</v>
+      </c>
+      <c r="F13" s="13">
+        <v>8.6607902779658685E-2</v>
+      </c>
+      <c r="G13" s="13">
+        <v>0</v>
+      </c>
+      <c r="H13" s="13">
+        <v>5.6139995515499898E-2</v>
+      </c>
+      <c r="I13" s="13">
+        <v>4.4405285933795755E-3</v>
+      </c>
+      <c r="J13" s="13">
+        <v>3.0313057049530415E-2</v>
+      </c>
+      <c r="K13" s="13">
+        <v>0</v>
+      </c>
+      <c r="L13" s="13">
+        <v>0</v>
+      </c>
+      <c r="M13" s="13">
+        <v>0</v>
+      </c>
+      <c r="N13" s="13">
+        <v>1.1390733787307098E-4</v>
+      </c>
+      <c r="O13" s="13">
+        <f t="shared" si="0"/>
+        <v>0.17761539127594161</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A14" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="F14" s="13">
+        <v>8.7459087373842489E-4</v>
+      </c>
+      <c r="G14" s="13">
+        <v>0</v>
+      </c>
+      <c r="H14" s="13">
+        <v>0.13053709997854207</v>
+      </c>
+      <c r="I14" s="13">
+        <v>4.4419226263729041E-3</v>
+      </c>
+      <c r="J14" s="13">
+        <v>2.1803377955088812E-2</v>
+      </c>
+      <c r="K14" s="13">
+        <v>1.1979539722724928E-2</v>
+      </c>
+      <c r="L14" s="13">
+        <v>0.14113769702903531</v>
+      </c>
+      <c r="M14" s="13">
+        <v>0</v>
+      </c>
+      <c r="N14" s="13">
+        <v>4.1203503914668971E-3</v>
+      </c>
+      <c r="O14" s="13">
+        <f t="shared" si="0"/>
+        <v>0.3148945785769694</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A15" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>247</v>
+      </c>
+      <c r="F15" s="13">
+        <v>1.17229497866177E-2</v>
+      </c>
+      <c r="G15" s="13">
+        <v>0</v>
+      </c>
+      <c r="H15" s="13">
+        <v>3.5769313585755406E-2</v>
+      </c>
+      <c r="I15" s="13">
+        <v>6.0203125526081388E-3</v>
+      </c>
+      <c r="J15" s="13">
+        <v>3.0484230282147957E-3</v>
+      </c>
+      <c r="K15" s="13">
+        <v>9.7858909837310659E-2</v>
+      </c>
+      <c r="L15" s="13">
+        <v>5.0392932257344182E-2</v>
+      </c>
+      <c r="M15" s="13">
+        <v>0</v>
+      </c>
+      <c r="N15" s="13">
+        <v>1.2206433975752797E-2</v>
+      </c>
+      <c r="O15" s="13">
+        <f t="shared" si="0"/>
+        <v>0.21701927502360369</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A16" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="F16" s="13">
+        <v>2.0360572040874696E-2</v>
+      </c>
+      <c r="G16" s="13">
+        <v>0</v>
+      </c>
+      <c r="H16" s="13">
+        <v>1.8048764805684719E-2</v>
+      </c>
+      <c r="I16" s="13">
+        <v>7.1080430253747773E-2</v>
+      </c>
+      <c r="J16" s="13">
+        <v>1.6794140430403264E-2</v>
+      </c>
+      <c r="K16" s="13">
+        <v>0.82946831133312526</v>
+      </c>
+      <c r="L16" s="13">
+        <v>0.16597962554575643</v>
+      </c>
+      <c r="M16" s="13">
+        <v>3.834136885883118E-2</v>
+      </c>
+      <c r="N16" s="13">
+        <v>7.1850181142675499E-3</v>
+      </c>
+      <c r="O16" s="13">
+        <f t="shared" si="0"/>
+        <v>1.1672582313826909</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A17" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="F17" s="13">
+        <v>3.1110461332016129E-2</v>
+      </c>
+      <c r="G17" s="13">
+        <v>0</v>
+      </c>
+      <c r="H17" s="13">
+        <v>9.8085810791392516E-2</v>
+      </c>
+      <c r="I17" s="13">
+        <v>6.2631881016417786E-3</v>
+      </c>
+      <c r="J17" s="13">
+        <v>1.2045762819983066E-2</v>
+      </c>
+      <c r="K17" s="13">
+        <v>0</v>
+      </c>
+      <c r="L17" s="13">
+        <v>4.939633167439577E-2</v>
+      </c>
+      <c r="M17" s="13">
+        <v>0</v>
+      </c>
+      <c r="N17" s="13">
+        <v>1.0216507837788628E-2</v>
+      </c>
+      <c r="O17" s="13">
+        <f t="shared" si="0"/>
+        <v>0.2071180625572179</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A18" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="F18" s="13">
+        <v>9.9156609860982575E-4</v>
+      </c>
+      <c r="G18" s="13">
+        <v>0</v>
+      </c>
+      <c r="H18" s="13">
+        <v>5.9600802078748891E-2</v>
+      </c>
+      <c r="I18" s="13">
+        <v>0.22296113826612415</v>
+      </c>
+      <c r="J18" s="13">
+        <v>1.459501032109661E-2</v>
+      </c>
+      <c r="K18" s="13">
+        <v>0</v>
+      </c>
+      <c r="L18" s="13">
+        <v>0</v>
+      </c>
+      <c r="M18" s="13">
+        <v>0</v>
+      </c>
+      <c r="N18" s="13">
+        <v>2.4997646469694504E-2</v>
+      </c>
+      <c r="O18" s="13">
+        <f t="shared" si="0"/>
+        <v>0.32314616323427398</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A19" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>263</v>
+      </c>
+      <c r="F19" s="13">
+        <v>1.7412883672319995E-2</v>
+      </c>
+      <c r="G19" s="13">
+        <v>0</v>
+      </c>
+      <c r="H19" s="13">
+        <v>2.6740075388712509E-2</v>
+      </c>
+      <c r="I19" s="13">
+        <v>6.6740477705370732E-3</v>
+      </c>
+      <c r="J19" s="13">
+        <v>7.1856261639111421E-3</v>
+      </c>
+      <c r="K19" s="13">
+        <v>0</v>
+      </c>
+      <c r="L19" s="13">
+        <v>0</v>
+      </c>
+      <c r="M19" s="13">
+        <v>0</v>
+      </c>
+      <c r="N19" s="13">
+        <v>3.0059656082891722E-2</v>
+      </c>
+      <c r="O19" s="13">
+        <f t="shared" si="0"/>
+        <v>8.8072289078372445E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A20" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="F20" s="13">
+        <v>5.4921736374614818E-4</v>
+      </c>
+      <c r="G20" s="13">
+        <v>0</v>
+      </c>
+      <c r="H20" s="13">
+        <v>1.5685693676201035E-3</v>
+      </c>
+      <c r="I20" s="13">
+        <v>2.5208928389398957E-3</v>
+      </c>
+      <c r="J20" s="13">
+        <v>5.0677318604055652E-3</v>
+      </c>
+      <c r="K20" s="13">
+        <v>0</v>
+      </c>
+      <c r="L20" s="13">
+        <v>0</v>
+      </c>
+      <c r="M20" s="13">
+        <v>0</v>
+      </c>
+      <c r="N20" s="13">
+        <v>5.9442369770925452E-3</v>
+      </c>
+      <c r="O20" s="13">
+        <f t="shared" si="0"/>
+        <v>1.5650648407804259E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A21" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="F21" s="13">
+        <v>1.5620925417579982E-2</v>
+      </c>
+      <c r="G21" s="13">
+        <v>0</v>
+      </c>
+      <c r="H21" s="13">
+        <v>8.6865807165920647E-4</v>
+      </c>
+      <c r="I21" s="13">
+        <v>0</v>
+      </c>
+      <c r="J21" s="13">
+        <v>0</v>
+      </c>
+      <c r="K21" s="13">
+        <v>0</v>
+      </c>
+      <c r="L21" s="13">
+        <v>0</v>
+      </c>
+      <c r="M21" s="13">
+        <v>0.10064609325443184</v>
+      </c>
+      <c r="N21" s="13">
+        <v>0</v>
+      </c>
+      <c r="O21" s="13">
+        <f t="shared" si="0"/>
+        <v>0.11713567674367104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A22" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="F22" s="13">
+        <v>3.4186178624074724E-3</v>
+      </c>
+      <c r="G22" s="13">
+        <v>0</v>
+      </c>
+      <c r="H22" s="13">
+        <v>0</v>
+      </c>
+      <c r="I22" s="13">
+        <v>0</v>
+      </c>
+      <c r="J22" s="13">
+        <v>9.9211254678497236E-3</v>
+      </c>
+      <c r="K22" s="13">
+        <v>0</v>
+      </c>
+      <c r="L22" s="13">
+        <v>0</v>
+      </c>
+      <c r="M22" s="13">
+        <v>0</v>
+      </c>
+      <c r="N22" s="13">
+        <v>0</v>
+      </c>
+      <c r="O22" s="13">
+        <f t="shared" si="0"/>
+        <v>1.3339743330257196E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A23" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="F23" s="13">
+        <v>2.7979038074110039E-2</v>
+      </c>
+      <c r="G23" s="13">
+        <v>0</v>
+      </c>
+      <c r="H23" s="13">
+        <v>2.5157760248967889E-2</v>
+      </c>
+      <c r="I23" s="13">
+        <v>1.2920491911561475E-2</v>
+      </c>
+      <c r="J23" s="13">
+        <v>8.565932346283698E-3</v>
+      </c>
+      <c r="K23" s="13">
+        <v>0</v>
+      </c>
+      <c r="L23" s="13">
+        <v>0</v>
+      </c>
+      <c r="M23" s="13">
+        <v>0</v>
+      </c>
+      <c r="N23" s="13">
+        <v>0</v>
+      </c>
+      <c r="O23" s="13">
+        <f t="shared" si="0"/>
+        <v>7.462322258092309E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A24" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="F24" s="13">
+        <v>6.6879028320133531E-3</v>
+      </c>
+      <c r="G24" s="13">
+        <v>0</v>
+      </c>
+      <c r="H24" s="13">
+        <v>3.3319631638462029E-2</v>
+      </c>
+      <c r="I24" s="13">
+        <v>4.7785894219920313E-3</v>
+      </c>
+      <c r="J24" s="13">
+        <v>1.7459385446217583E-5</v>
+      </c>
+      <c r="K24" s="13">
+        <v>0</v>
+      </c>
+      <c r="L24" s="13">
+        <v>0</v>
+      </c>
+      <c r="M24" s="13">
+        <v>0</v>
+      </c>
+      <c r="N24" s="13">
+        <v>0</v>
+      </c>
+      <c r="O24" s="13">
+        <f t="shared" si="0"/>
+        <v>4.4803583277913631E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A25" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>209</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="F25" s="13">
+        <v>3.6603642548046966E-3</v>
+      </c>
+      <c r="G25" s="13">
+        <v>0</v>
+      </c>
+      <c r="H25" s="13">
+        <v>2.3169239608589236E-2</v>
+      </c>
+      <c r="I25" s="13">
+        <v>2.0188985202985264E-3</v>
+      </c>
+      <c r="J25" s="13">
+        <v>3.4918770892435167E-5</v>
+      </c>
+      <c r="K25" s="13">
+        <v>1.2546014081706493E-3</v>
+      </c>
+      <c r="L25" s="13">
+        <v>0</v>
+      </c>
+      <c r="M25" s="13">
+        <v>0</v>
+      </c>
+      <c r="N25" s="13">
+        <v>5.3129952237446383E-3</v>
+      </c>
+      <c r="O25" s="13">
+        <f t="shared" si="0"/>
+        <v>3.5451017786500186E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A26" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>213</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>214</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>259</v>
+      </c>
+      <c r="F26" s="13">
+        <v>1.4214584387352359E-2</v>
+      </c>
+      <c r="G26" s="13">
+        <v>0</v>
+      </c>
+      <c r="H26" s="13">
+        <v>3.008567342703862E-2</v>
+      </c>
+      <c r="I26" s="13">
+        <v>1.2152955813955044E-3</v>
+      </c>
+      <c r="J26" s="13">
+        <v>0</v>
+      </c>
+      <c r="K26" s="13">
+        <v>0</v>
+      </c>
+      <c r="L26" s="13">
+        <v>0</v>
+      </c>
+      <c r="M26" s="13">
+        <v>0</v>
+      </c>
+      <c r="N26" s="13">
+        <v>0</v>
+      </c>
+      <c r="O26" s="13">
+        <f t="shared" si="0"/>
+        <v>4.5515553395786487E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A27" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>214</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="F27" s="13">
+        <v>2.7970192529336677E-2</v>
+      </c>
+      <c r="G27" s="13">
+        <v>0</v>
+      </c>
+      <c r="H27" s="13">
+        <v>0</v>
+      </c>
+      <c r="I27" s="13">
+        <v>1.4766180490810072E-4</v>
+      </c>
+      <c r="J27" s="13">
+        <v>0</v>
+      </c>
+      <c r="K27" s="13">
+        <v>0</v>
+      </c>
+      <c r="L27" s="13">
+        <v>0</v>
+      </c>
+      <c r="M27" s="13">
+        <v>0</v>
+      </c>
+      <c r="N27" s="13">
+        <v>0</v>
+      </c>
+      <c r="O27" s="13">
+        <f t="shared" si="0"/>
+        <v>2.8117854334244779E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A28" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>218</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>214</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>258</v>
+      </c>
+      <c r="F28" s="13">
+        <v>1.7555222694894512E-2</v>
+      </c>
+      <c r="G28" s="13">
+        <v>1.6402222396709361E-2</v>
+      </c>
+      <c r="H28" s="13">
+        <v>2.8292940673136757E-2</v>
+      </c>
+      <c r="I28" s="13">
+        <v>0</v>
+      </c>
+      <c r="J28" s="13">
+        <v>6.1756753205758746E-5</v>
+      </c>
+      <c r="K28" s="13">
+        <v>0</v>
+      </c>
+      <c r="L28" s="13">
+        <v>0</v>
+      </c>
+      <c r="M28" s="13">
+        <v>0</v>
+      </c>
+      <c r="N28" s="13">
+        <v>0</v>
+      </c>
+      <c r="O28" s="13">
+        <f t="shared" si="0"/>
+        <v>6.2312142517946388E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A29" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>231</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>231</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>231</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>231</v>
+      </c>
+      <c r="F29" s="13">
+        <v>0</v>
+      </c>
+      <c r="G29" s="13">
+        <v>0</v>
+      </c>
+      <c r="H29" s="13">
+        <v>2.0992159192780357E-2</v>
+      </c>
+      <c r="I29" s="13">
+        <v>2.0758180541572979E-2</v>
+      </c>
+      <c r="J29" s="13">
+        <v>9.1702544696565681E-3</v>
+      </c>
+      <c r="K29" s="13">
+        <v>0</v>
+      </c>
+      <c r="L29" s="13">
+        <v>0</v>
+      </c>
+      <c r="M29" s="13">
+        <v>0</v>
+      </c>
+      <c r="N29" s="13">
+        <v>8.5619718251768485E-3</v>
+      </c>
+      <c r="O29" s="13">
+        <f t="shared" si="0"/>
+        <v>5.9482566029186751E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A30" s="14" t="s">
+        <v>232</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>233</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>233</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>234</v>
+      </c>
+      <c r="E30" s="14" t="s">
+        <v>233</v>
+      </c>
+      <c r="F30" s="13">
+        <v>7.688473554779842E-4</v>
+      </c>
+      <c r="G30" s="13">
+        <v>0</v>
+      </c>
+      <c r="H30" s="13">
+        <v>7.3061497836180139E-4</v>
+      </c>
+      <c r="I30" s="13">
+        <v>1.8736331086805754E-3</v>
+      </c>
+      <c r="J30" s="13">
+        <v>9.8182227369926121E-4</v>
+      </c>
+      <c r="K30" s="13">
+        <v>2.6198355681992285E-2</v>
+      </c>
+      <c r="L30" s="13">
+        <v>0</v>
+      </c>
+      <c r="M30" s="13">
+        <v>0</v>
+      </c>
+      <c r="N30" s="13">
+        <v>5.0320667221219802E-3</v>
+      </c>
+      <c r="O30" s="13">
+        <f t="shared" si="0"/>
+        <v>3.5585340120333889E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A31" s="14" t="s">
+        <v>235</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>237</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E31" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="F31" s="13">
+        <v>2.1315767135029879E-2</v>
+      </c>
+      <c r="G31" s="13">
+        <v>0</v>
+      </c>
+      <c r="H31" s="13">
+        <v>1.7316880703924998E-2</v>
+      </c>
+      <c r="I31" s="13">
+        <v>0.42407830134690239</v>
+      </c>
+      <c r="J31" s="13">
+        <v>6.2277129008866457E-2</v>
+      </c>
+      <c r="K31" s="13">
+        <v>2.5092028163412987E-3</v>
+      </c>
+      <c r="L31" s="13">
+        <v>0</v>
+      </c>
+      <c r="M31" s="13">
+        <v>0</v>
+      </c>
+      <c r="N31" s="13">
+        <v>0.59411795865154682</v>
+      </c>
+      <c r="O31" s="13">
+        <f t="shared" si="0"/>
+        <v>1.1216152396626118</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A32" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="E32" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="F32" s="13">
+        <v>2.1199282006619941E-3</v>
+      </c>
+      <c r="G32" s="13">
+        <v>0</v>
+      </c>
+      <c r="H32" s="13">
+        <v>6.7450512619343624E-3</v>
+      </c>
+      <c r="I32" s="13">
+        <v>6.0424588311166968E-2</v>
+      </c>
+      <c r="J32" s="13">
+        <v>6.5719982823656811E-3</v>
+      </c>
+      <c r="K32" s="13">
+        <v>2.1746424408291255E-2</v>
+      </c>
+      <c r="L32" s="13">
+        <v>0.24698165837197883</v>
+      </c>
+      <c r="M32" s="13">
+        <v>0</v>
+      </c>
+      <c r="N32" s="13">
+        <v>0.20975693617531671</v>
+      </c>
+      <c r="O32" s="13">
+        <f t="shared" si="0"/>
+        <v>0.55434658501171574</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A33" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>243</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>242</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>243</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F33" s="13">
+        <v>7.5247704455136732E-2</v>
+      </c>
+      <c r="G33" s="13">
+        <v>4.6324627298181979E-2</v>
+      </c>
+      <c r="H33" s="13">
+        <v>2.7432580514912774E-2</v>
+      </c>
+      <c r="I33" s="13">
+        <v>4.2851334034672617E-2</v>
+      </c>
+      <c r="J33" s="13">
+        <v>0.40318513080347368</v>
+      </c>
+      <c r="K33" s="13">
+        <v>0</v>
+      </c>
+      <c r="L33" s="13">
+        <v>9.879266334879154E-2</v>
+      </c>
+      <c r="M33" s="13">
+        <v>2.8756026644123387E-2</v>
+      </c>
+      <c r="N33" s="13">
+        <v>4.996409501514168E-2</v>
+      </c>
+      <c r="O33" s="13">
+        <f t="shared" si="0"/>
+        <v>0.7725541621144344</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB4D6698-6C84-478E-9876-63A69E078122}">
+  <dimension ref="A1:O33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="5" max="5" width="27.1328125" customWidth="1"/>
+    <col min="6" max="6" width="25.36328125" customWidth="1"/>
+    <col min="7" max="15" width="12.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A1" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" t="s">
+        <v>248</v>
+      </c>
+      <c r="O1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B2" t="s">
+        <v>250</v>
+      </c>
+      <c r="C2" t="s">
+        <v>213</v>
+      </c>
+      <c r="D2" t="s">
+        <v>250</v>
+      </c>
+      <c r="E2" t="s">
+        <v>250</v>
+      </c>
+      <c r="F2" s="15">
+        <f>Tabelle1!F2/Tabelle1!$O2</f>
+        <v>0.36244410666248883</v>
+      </c>
+      <c r="G2" s="15">
+        <f>Tabelle1!G2/Tabelle1!$O2</f>
+        <v>4.0058380182997075E-3</v>
+      </c>
+      <c r="H2" s="15">
+        <f>Tabelle1!H2/Tabelle1!$O2</f>
+        <v>0.49899912068580149</v>
+      </c>
+      <c r="I2" s="15">
+        <f>Tabelle1!I2/Tabelle1!$O2</f>
+        <v>7.6161273468584645E-2</v>
+      </c>
+      <c r="J2" s="15">
+        <f>Tabelle1!J2/Tabelle1!$O2</f>
+        <v>5.8389661164825378E-2</v>
+      </c>
+      <c r="K2" s="15">
+        <f>Tabelle1!K2/Tabelle1!$O2</f>
+        <v>0</v>
+      </c>
+      <c r="L2" s="15">
+        <f>Tabelle1!L2/Tabelle1!$O2</f>
+        <v>0</v>
+      </c>
+      <c r="M2" s="15">
+        <f>Tabelle1!M2/Tabelle1!$O2</f>
+        <v>0</v>
+      </c>
+      <c r="N2" s="15">
+        <f>Tabelle1!N2/Tabelle1!$O2</f>
+        <v>0</v>
+      </c>
+      <c r="O2" s="13">
+        <f>SUM(F2:N2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A3" t="s">
+        <v>223</v>
+      </c>
+      <c r="B3" t="s">
+        <v>251</v>
+      </c>
+      <c r="C3" t="s">
+        <v>192</v>
+      </c>
+      <c r="D3" t="s">
+        <v>251</v>
+      </c>
+      <c r="E3" t="s">
+        <v>251</v>
+      </c>
+      <c r="F3" s="15">
+        <f>Tabelle1!F3/Tabelle1!$O3</f>
+        <v>0.35239435886166059</v>
+      </c>
+      <c r="G3" s="15">
+        <f>Tabelle1!G3/Tabelle1!$O3</f>
+        <v>0</v>
+      </c>
+      <c r="H3" s="15">
+        <f>Tabelle1!H3/Tabelle1!$O3</f>
+        <v>0.43879888515990734</v>
+      </c>
+      <c r="I3" s="15">
+        <f>Tabelle1!I3/Tabelle1!$O3</f>
+        <v>0.2077616460058693</v>
+      </c>
+      <c r="J3" s="15">
+        <f>Tabelle1!J3/Tabelle1!$O3</f>
+        <v>1.0451099725627428E-3</v>
+      </c>
+      <c r="K3" s="15">
+        <f>Tabelle1!K3/Tabelle1!$O3</f>
+        <v>0</v>
+      </c>
+      <c r="L3" s="15">
+        <f>Tabelle1!L3/Tabelle1!$O3</f>
+        <v>0</v>
+      </c>
+      <c r="M3" s="15">
+        <f>Tabelle1!M3/Tabelle1!$O3</f>
+        <v>0</v>
+      </c>
+      <c r="N3" s="15">
+        <f>Tabelle1!N3/Tabelle1!$O3</f>
+        <v>0</v>
+      </c>
+      <c r="O3" s="13">
+        <f t="shared" ref="O3:O33" si="0">SUM(F3:N3)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A4" t="s">
+        <v>224</v>
+      </c>
+      <c r="B4" t="s">
+        <v>252</v>
+      </c>
+      <c r="C4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4" t="s">
+        <v>252</v>
+      </c>
+      <c r="E4" t="s">
+        <v>252</v>
+      </c>
+      <c r="F4" s="15">
+        <f>Tabelle1!F4/Tabelle1!$O4</f>
+        <v>0.23292684502960961</v>
+      </c>
+      <c r="G4" s="15">
+        <f>Tabelle1!G4/Tabelle1!$O4</f>
+        <v>1.0500967709564035E-3</v>
+      </c>
+      <c r="H4" s="15">
+        <f>Tabelle1!H4/Tabelle1!$O4</f>
+        <v>0.40446242394705129</v>
+      </c>
+      <c r="I4" s="15">
+        <f>Tabelle1!I4/Tabelle1!$O4</f>
+        <v>9.5189204363291674E-2</v>
+      </c>
+      <c r="J4" s="15">
+        <f>Tabelle1!J4/Tabelle1!$O4</f>
+        <v>0.25370976779906251</v>
+      </c>
+      <c r="K4" s="15">
+        <f>Tabelle1!K4/Tabelle1!$O4</f>
+        <v>0</v>
+      </c>
+      <c r="L4" s="15">
+        <f>Tabelle1!L4/Tabelle1!$O4</f>
+        <v>1.2661662090028468E-2</v>
+      </c>
+      <c r="M4" s="15">
+        <f>Tabelle1!M4/Tabelle1!$O4</f>
+        <v>0</v>
+      </c>
+      <c r="N4" s="15">
+        <f>Tabelle1!N4/Tabelle1!$O4</f>
+        <v>0</v>
+      </c>
+      <c r="O4" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A5" t="s">
+        <v>226</v>
+      </c>
+      <c r="B5" t="s">
+        <v>253</v>
+      </c>
+      <c r="C5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" t="s">
+        <v>253</v>
+      </c>
+      <c r="E5" t="s">
+        <v>253</v>
+      </c>
+      <c r="F5" s="15">
+        <f>Tabelle1!F5/Tabelle1!$O5</f>
+        <v>0.16092555867402636</v>
+      </c>
+      <c r="G5" s="15">
+        <f>Tabelle1!G5/Tabelle1!$O5</f>
+        <v>3.4656942954268055E-3</v>
+      </c>
+      <c r="H5" s="15">
+        <f>Tabelle1!H5/Tabelle1!$O5</f>
+        <v>0.10387604084164948</v>
+      </c>
+      <c r="I5" s="15">
+        <f>Tabelle1!I5/Tabelle1!$O5</f>
+        <v>2.7929928177684405E-2</v>
+      </c>
+      <c r="J5" s="15">
+        <f>Tabelle1!J5/Tabelle1!$O5</f>
+        <v>0.70380277801121294</v>
+      </c>
+      <c r="K5" s="15">
+        <f>Tabelle1!K5/Tabelle1!$O5</f>
+        <v>0</v>
+      </c>
+      <c r="L5" s="15">
+        <f>Tabelle1!L5/Tabelle1!$O5</f>
+        <v>0</v>
+      </c>
+      <c r="M5" s="15">
+        <f>Tabelle1!M5/Tabelle1!$O5</f>
+        <v>0</v>
+      </c>
+      <c r="N5" s="15">
+        <f>Tabelle1!N5/Tabelle1!$O5</f>
+        <v>0</v>
+      </c>
+      <c r="O5" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A6" t="s">
+        <v>227</v>
+      </c>
+      <c r="B6" t="s">
+        <v>254</v>
+      </c>
+      <c r="C6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D6" t="s">
+        <v>254</v>
+      </c>
+      <c r="E6" t="s">
+        <v>254</v>
+      </c>
+      <c r="F6" s="15">
+        <f>Tabelle1!F6/Tabelle1!$O6</f>
+        <v>0.40753041534452816</v>
+      </c>
+      <c r="G6" s="15">
+        <f>Tabelle1!G6/Tabelle1!$O6</f>
+        <v>2.9318248516149066E-3</v>
+      </c>
+      <c r="H6" s="15">
+        <f>Tabelle1!H6/Tabelle1!$O6</f>
+        <v>0.18565057422404219</v>
+      </c>
+      <c r="I6" s="15">
+        <f>Tabelle1!I6/Tabelle1!$O6</f>
+        <v>2.4773554339729102E-2</v>
+      </c>
+      <c r="J6" s="15">
+        <f>Tabelle1!J6/Tabelle1!$O6</f>
+        <v>0.37911363124008568</v>
+      </c>
+      <c r="K6" s="15">
+        <f>Tabelle1!K6/Tabelle1!$O6</f>
+        <v>0</v>
+      </c>
+      <c r="L6" s="15">
+        <f>Tabelle1!L6/Tabelle1!$O6</f>
+        <v>0</v>
+      </c>
+      <c r="M6" s="15">
+        <f>Tabelle1!M6/Tabelle1!$O6</f>
+        <v>0</v>
+      </c>
+      <c r="N6" s="15">
+        <f>Tabelle1!N6/Tabelle1!$O6</f>
+        <v>0</v>
+      </c>
+      <c r="O6" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A7" t="s">
+        <v>225</v>
+      </c>
+      <c r="B7" t="s">
+        <v>255</v>
+      </c>
+      <c r="C7" t="s">
+        <v>192</v>
+      </c>
+      <c r="D7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E7" t="s">
+        <v>255</v>
+      </c>
+      <c r="F7" s="15">
+        <f>Tabelle1!F7/Tabelle1!$O7</f>
+        <v>8.1625819411281983E-2</v>
+      </c>
+      <c r="G7" s="15">
+        <f>Tabelle1!G7/Tabelle1!$O7</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="15">
+        <f>Tabelle1!H7/Tabelle1!$O7</f>
+        <v>0.54158894721480944</v>
+      </c>
+      <c r="I7" s="15">
+        <f>Tabelle1!I7/Tabelle1!$O7</f>
+        <v>0.27741666882137689</v>
+      </c>
+      <c r="J7" s="15">
+        <f>Tabelle1!J7/Tabelle1!$O7</f>
+        <v>9.9368564552531777E-2</v>
+      </c>
+      <c r="K7" s="15">
+        <f>Tabelle1!K7/Tabelle1!$O7</f>
+        <v>0</v>
+      </c>
+      <c r="L7" s="15">
+        <f>Tabelle1!L7/Tabelle1!$O7</f>
+        <v>0</v>
+      </c>
+      <c r="M7" s="15">
+        <f>Tabelle1!M7/Tabelle1!$O7</f>
+        <v>0</v>
+      </c>
+      <c r="N7" s="15">
+        <f>Tabelle1!N7/Tabelle1!$O7</f>
+        <v>0</v>
+      </c>
+      <c r="O7" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" s="15">
+        <f>Tabelle1!F8/Tabelle1!$O8</f>
+        <v>2.0392315246833988E-2</v>
+      </c>
+      <c r="G8" s="15">
+        <f>Tabelle1!G8/Tabelle1!$O8</f>
+        <v>0.39816168942102231</v>
+      </c>
+      <c r="H8" s="15">
+        <f>Tabelle1!H8/Tabelle1!$O8</f>
+        <v>1.6265866731395424E-2</v>
+      </c>
+      <c r="I8" s="15">
+        <f>Tabelle1!I8/Tabelle1!$O8</f>
+        <v>8.6068448681967031E-4</v>
+      </c>
+      <c r="J8" s="15">
+        <f>Tabelle1!J8/Tabelle1!$O8</f>
+        <v>3.80667369771246E-2</v>
+      </c>
+      <c r="K8" s="15">
+        <f>Tabelle1!K8/Tabelle1!$O8</f>
+        <v>0</v>
+      </c>
+      <c r="L8" s="15">
+        <f>Tabelle1!L8/Tabelle1!$O8</f>
+        <v>0</v>
+      </c>
+      <c r="M8" s="15">
+        <f>Tabelle1!M8/Tabelle1!$O8</f>
+        <v>0.52625270713680394</v>
+      </c>
+      <c r="N8" s="15">
+        <f>Tabelle1!N8/Tabelle1!$O8</f>
+        <v>0</v>
+      </c>
+      <c r="O8" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" t="s">
+        <v>71</v>
+      </c>
+      <c r="F9" s="15">
+        <f>Tabelle1!F9/Tabelle1!$O9</f>
+        <v>0.45114079793505762</v>
+      </c>
+      <c r="G9" s="15">
+        <f>Tabelle1!G9/Tabelle1!$O9</f>
+        <v>0.26825118155964772</v>
+      </c>
+      <c r="H9" s="15">
+        <f>Tabelle1!H9/Tabelle1!$O9</f>
+        <v>3.8262895298749315E-2</v>
+      </c>
+      <c r="I9" s="15">
+        <f>Tabelle1!I9/Tabelle1!$O9</f>
+        <v>0</v>
+      </c>
+      <c r="J9" s="15">
+        <f>Tabelle1!J9/Tabelle1!$O9</f>
+        <v>8.4030595819138134E-4</v>
+      </c>
+      <c r="K9" s="15">
+        <f>Tabelle1!K9/Tabelle1!$O9</f>
+        <v>0</v>
+      </c>
+      <c r="L9" s="15">
+        <f>Tabelle1!L9/Tabelle1!$O9</f>
+        <v>0</v>
+      </c>
+      <c r="M9" s="15">
+        <f>Tabelle1!M9/Tabelle1!$O9</f>
+        <v>0.24150481924835399</v>
+      </c>
+      <c r="N9" s="15">
+        <f>Tabelle1!N9/Tabelle1!$O9</f>
+        <v>0</v>
+      </c>
+      <c r="O9" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" t="s">
+        <v>74</v>
+      </c>
+      <c r="F10" s="15">
+        <f>Tabelle1!F10/Tabelle1!$O10</f>
+        <v>0.51268870890691032</v>
+      </c>
+      <c r="G10" s="15">
+        <f>Tabelle1!G10/Tabelle1!$O10</f>
+        <v>0.11004694156674071</v>
+      </c>
+      <c r="H10" s="15">
+        <f>Tabelle1!H10/Tabelle1!$O10</f>
+        <v>0.34405301848383918</v>
+      </c>
+      <c r="I10" s="15">
+        <f>Tabelle1!I10/Tabelle1!$O10</f>
+        <v>0</v>
+      </c>
+      <c r="J10" s="15">
+        <f>Tabelle1!J10/Tabelle1!$O10</f>
+        <v>1.5976860931695737E-2</v>
+      </c>
+      <c r="K10" s="15">
+        <f>Tabelle1!K10/Tabelle1!$O10</f>
+        <v>0</v>
+      </c>
+      <c r="L10" s="15">
+        <f>Tabelle1!L10/Tabelle1!$O10</f>
+        <v>1.7234470110814169E-2</v>
+      </c>
+      <c r="M10" s="15">
+        <f>Tabelle1!M10/Tabelle1!$O10</f>
+        <v>0</v>
+      </c>
+      <c r="N10" s="15">
+        <f>Tabelle1!N10/Tabelle1!$O10</f>
+        <v>0</v>
+      </c>
+      <c r="O10" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A11" t="s">
+        <v>106</v>
+      </c>
+      <c r="B11" t="s">
+        <v>107</v>
+      </c>
+      <c r="C11" t="s">
+        <v>102</v>
+      </c>
+      <c r="D11" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" t="s">
+        <v>244</v>
+      </c>
+      <c r="F11" s="15">
+        <f>Tabelle1!F11/Tabelle1!$O11</f>
+        <v>0.69140741245293658</v>
+      </c>
+      <c r="G11" s="15">
+        <f>Tabelle1!G11/Tabelle1!$O11</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="15">
+        <f>Tabelle1!H11/Tabelle1!$O11</f>
+        <v>0.16606144990787414</v>
+      </c>
+      <c r="I11" s="15">
+        <f>Tabelle1!I11/Tabelle1!$O11</f>
+        <v>2.2112559505588325E-2</v>
+      </c>
+      <c r="J11" s="15">
+        <f>Tabelle1!J11/Tabelle1!$O11</f>
+        <v>3.9971001978331484E-2</v>
+      </c>
+      <c r="K11" s="15">
+        <f>Tabelle1!K11/Tabelle1!$O11</f>
+        <v>0</v>
+      </c>
+      <c r="L11" s="15">
+        <f>Tabelle1!L11/Tabelle1!$O11</f>
+        <v>0</v>
+      </c>
+      <c r="M11" s="15">
+        <f>Tabelle1!M11/Tabelle1!$O11</f>
+        <v>4.1690304051216549E-2</v>
+      </c>
+      <c r="N11" s="15">
+        <f>Tabelle1!N11/Tabelle1!$O11</f>
+        <v>3.8757272104052935E-2</v>
+      </c>
+      <c r="O11" s="13">
+        <f t="shared" si="0"/>
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A12" t="s">
+        <v>119</v>
+      </c>
+      <c r="B12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C12" t="s">
+        <v>102</v>
+      </c>
+      <c r="D12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E12" t="s">
+        <v>245</v>
+      </c>
+      <c r="F12" s="15">
+        <f>Tabelle1!F12/Tabelle1!$O12</f>
+        <v>1.9628842267901452E-2</v>
+      </c>
+      <c r="G12" s="15">
+        <f>Tabelle1!G12/Tabelle1!$O12</f>
+        <v>0</v>
+      </c>
+      <c r="H12" s="15">
+        <f>Tabelle1!H12/Tabelle1!$O12</f>
+        <v>4.786615535210749E-2</v>
+      </c>
+      <c r="I12" s="15">
+        <f>Tabelle1!I12/Tabelle1!$O12</f>
+        <v>3.2355608218323839E-2</v>
+      </c>
+      <c r="J12" s="15">
+        <f>Tabelle1!J12/Tabelle1!$O12</f>
+        <v>0.571470121137582</v>
+      </c>
+      <c r="K12" s="15">
+        <f>Tabelle1!K12/Tabelle1!$O12</f>
+        <v>0</v>
+      </c>
+      <c r="L12" s="15">
+        <f>Tabelle1!L12/Tabelle1!$O12</f>
+        <v>0.32867927302408534</v>
+      </c>
+      <c r="M12" s="15">
+        <f>Tabelle1!M12/Tabelle1!$O12</f>
+        <v>0</v>
+      </c>
+      <c r="N12" s="15">
+        <f>Tabelle1!N12/Tabelle1!$O12</f>
+        <v>0</v>
+      </c>
+      <c r="O12" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A13" t="s">
+        <v>121</v>
+      </c>
+      <c r="B13" t="s">
+        <v>122</v>
+      </c>
+      <c r="C13" t="s">
+        <v>102</v>
+      </c>
+      <c r="D13" t="s">
+        <v>75</v>
+      </c>
+      <c r="E13" t="s">
+        <v>246</v>
+      </c>
+      <c r="F13" s="15">
+        <f>Tabelle1!F13/Tabelle1!$O13</f>
+        <v>0.48761485227992124</v>
+      </c>
+      <c r="G13" s="15">
+        <f>Tabelle1!G13/Tabelle1!$O13</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="15">
+        <f>Tabelle1!H13/Tabelle1!$O13</f>
+        <v>0.31607618637216706</v>
+      </c>
+      <c r="I13" s="15">
+        <f>Tabelle1!I13/Tabelle1!$O13</f>
+        <v>2.5000809679161261E-2</v>
+      </c>
+      <c r="J13" s="15">
+        <f>Tabelle1!J13/Tabelle1!$O13</f>
+        <v>0.17066683710105018</v>
+      </c>
+      <c r="K13" s="15">
+        <f>Tabelle1!K13/Tabelle1!$O13</f>
+        <v>0</v>
+      </c>
+      <c r="L13" s="15">
+        <f>Tabelle1!L13/Tabelle1!$O13</f>
+        <v>0</v>
+      </c>
+      <c r="M13" s="15">
+        <f>Tabelle1!M13/Tabelle1!$O13</f>
+        <v>0</v>
+      </c>
+      <c r="N13" s="15">
+        <f>Tabelle1!N13/Tabelle1!$O13</f>
+        <v>6.4131456770041742E-4</v>
+      </c>
+      <c r="O13" s="13">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A14" t="s">
+        <v>126</v>
+      </c>
+      <c r="B14" t="s">
+        <v>127</v>
+      </c>
+      <c r="C14" t="s">
+        <v>127</v>
+      </c>
+      <c r="D14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" t="s">
+        <v>127</v>
+      </c>
+      <c r="F14" s="15">
+        <f>Tabelle1!F14/Tabelle1!$O14</f>
+        <v>2.7774084828349923E-3</v>
+      </c>
+      <c r="G14" s="15">
+        <f>Tabelle1!G14/Tabelle1!$O14</f>
+        <v>0</v>
+      </c>
+      <c r="H14" s="15">
+        <f>Tabelle1!H14/Tabelle1!$O14</f>
+        <v>0.41454222733350427</v>
+      </c>
+      <c r="I14" s="15">
+        <f>Tabelle1!I14/Tabelle1!$O14</f>
+        <v>1.4106062563688022E-2</v>
+      </c>
+      <c r="J14" s="15">
+        <f>Tabelle1!J14/Tabelle1!$O14</f>
+        <v>6.9240245588284816E-2</v>
+      </c>
+      <c r="K14" s="15">
+        <f>Tabelle1!K14/Tabelle1!$O14</f>
+        <v>3.8043016735509722E-2</v>
+      </c>
+      <c r="L14" s="15">
+        <f>Tabelle1!L14/Tabelle1!$O14</f>
+        <v>0.44820618273851021</v>
+      </c>
+      <c r="M14" s="15">
+        <f>Tabelle1!M14/Tabelle1!$O14</f>
+        <v>0</v>
+      </c>
+      <c r="N14" s="15">
+        <f>Tabelle1!N14/Tabelle1!$O14</f>
+        <v>1.3084856557667803E-2</v>
+      </c>
+      <c r="O14" s="13">
+        <f t="shared" si="0"/>
+        <v>0.99999999999999978</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A15" t="s">
+        <v>140</v>
+      </c>
+      <c r="B15" t="s">
+        <v>141</v>
+      </c>
+      <c r="C15" t="s">
+        <v>142</v>
+      </c>
+      <c r="D15" t="s">
+        <v>75</v>
+      </c>
+      <c r="E15" t="s">
+        <v>266</v>
+      </c>
+      <c r="F15" s="15">
+        <f>Tabelle1!F15/Tabelle1!$O15</f>
+        <v>5.4018011927017433E-2</v>
+      </c>
+      <c r="G15" s="15">
+        <f>Tabelle1!G15/Tabelle1!$O15</f>
+        <v>0</v>
+      </c>
+      <c r="H15" s="15">
+        <f>Tabelle1!H15/Tabelle1!$O15</f>
+        <v>0.16482090626219734</v>
+      </c>
+      <c r="I15" s="15">
+        <f>Tabelle1!I15/Tabelle1!$O15</f>
+        <v>2.7740911732164579E-2</v>
+      </c>
+      <c r="J15" s="15">
+        <f>Tabelle1!J15/Tabelle1!$O15</f>
+        <v>1.4046784682527576E-2</v>
+      </c>
+      <c r="K15" s="15">
+        <f>Tabelle1!K15/Tabelle1!$O15</f>
+        <v>0.45092266494147687</v>
+      </c>
+      <c r="L15" s="15">
+        <f>Tabelle1!L15/Tabelle1!$O15</f>
+        <v>0.23220486867750936</v>
+      </c>
+      <c r="M15" s="15">
+        <f>Tabelle1!M15/Tabelle1!$O15</f>
+        <v>0</v>
+      </c>
+      <c r="N15" s="15">
+        <f>Tabelle1!N15/Tabelle1!$O15</f>
+        <v>5.6245851777106837E-2</v>
+      </c>
+      <c r="O15" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A16" t="s">
+        <v>147</v>
+      </c>
+      <c r="B16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C16" t="s">
+        <v>149</v>
+      </c>
+      <c r="D16" t="s">
+        <v>75</v>
+      </c>
+      <c r="E16" t="s">
+        <v>148</v>
+      </c>
+      <c r="F16" s="15">
+        <f>Tabelle1!F16/Tabelle1!$O16</f>
+        <v>1.7443074285932701E-2</v>
+      </c>
+      <c r="G16" s="15">
+        <f>Tabelle1!G16/Tabelle1!$O16</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="15">
+        <f>Tabelle1!H16/Tabelle1!$O16</f>
+        <v>1.5462529473281006E-2</v>
+      </c>
+      <c r="I16" s="15">
+        <f>Tabelle1!I16/Tabelle1!$O16</f>
+        <v>6.0895205827375939E-2</v>
+      </c>
+      <c r="J16" s="15">
+        <f>Tabelle1!J16/Tabelle1!$O16</f>
+        <v>1.4387682158822343E-2</v>
+      </c>
+      <c r="K16" s="15">
+        <f>Tabelle1!K16/Tabelle1!$O16</f>
+        <v>0.71061251832044725</v>
+      </c>
+      <c r="L16" s="15">
+        <f>Tabelle1!L16/Tabelle1!$O16</f>
+        <v>0.14219614913243586</v>
+      </c>
+      <c r="M16" s="15">
+        <f>Tabelle1!M16/Tabelle1!$O16</f>
+        <v>3.2847375009224321E-2</v>
+      </c>
+      <c r="N16" s="15">
+        <f>Tabelle1!N16/Tabelle1!$O16</f>
+        <v>6.1554657924805922E-3</v>
+      </c>
+      <c r="O16" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A17" t="s">
+        <v>150</v>
+      </c>
+      <c r="B17" t="s">
+        <v>151</v>
+      </c>
+      <c r="C17" t="s">
+        <v>151</v>
+      </c>
+      <c r="D17" t="s">
+        <v>75</v>
+      </c>
+      <c r="E17" t="s">
+        <v>151</v>
+      </c>
+      <c r="F17" s="15">
+        <f>Tabelle1!F17/Tabelle1!$O17</f>
+        <v>0.15020641342384919</v>
+      </c>
+      <c r="G17" s="15">
+        <f>Tabelle1!G17/Tabelle1!$O17</f>
+        <v>0</v>
+      </c>
+      <c r="H17" s="15">
+        <f>Tabelle1!H17/Tabelle1!$O17</f>
+        <v>0.47357439317633432</v>
+      </c>
+      <c r="I17" s="15">
+        <f>Tabelle1!I17/Tabelle1!$O17</f>
+        <v>3.0239700122298731E-2</v>
+      </c>
+      <c r="J17" s="15">
+        <f>Tabelle1!J17/Tabelle1!$O17</f>
+        <v>5.8158919947676385E-2</v>
+      </c>
+      <c r="K17" s="15">
+        <f>Tabelle1!K17/Tabelle1!$O17</f>
+        <v>0</v>
+      </c>
+      <c r="L17" s="15">
+        <f>Tabelle1!L17/Tabelle1!$O17</f>
+        <v>0.23849359666904796</v>
+      </c>
+      <c r="M17" s="15">
+        <f>Tabelle1!M17/Tabelle1!$O17</f>
+        <v>0</v>
+      </c>
+      <c r="N17" s="15">
+        <f>Tabelle1!N17/Tabelle1!$O17</f>
+        <v>4.9326976660793366E-2</v>
+      </c>
+      <c r="O17" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A18" t="s">
+        <v>152</v>
+      </c>
+      <c r="B18" t="s">
+        <v>153</v>
+      </c>
+      <c r="C18" t="s">
+        <v>154</v>
+      </c>
+      <c r="D18" t="s">
+        <v>75</v>
+      </c>
+      <c r="E18" t="s">
+        <v>153</v>
+      </c>
+      <c r="F18" s="15">
+        <f>Tabelle1!F18/Tabelle1!$O18</f>
+        <v>3.0684755427251098E-3</v>
+      </c>
+      <c r="G18" s="15">
+        <f>Tabelle1!G18/Tabelle1!$O18</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="15">
+        <f>Tabelle1!H18/Tabelle1!$O18</f>
+        <v>0.18443914506742759</v>
+      </c>
+      <c r="I18" s="15">
+        <f>Tabelle1!I18/Tabelle1!$O18</f>
+        <v>0.68996993816845087</v>
+      </c>
+      <c r="J18" s="15">
+        <f>Tabelle1!J18/Tabelle1!$O18</f>
+        <v>4.51653523440275E-2</v>
+      </c>
+      <c r="K18" s="15">
+        <f>Tabelle1!K18/Tabelle1!$O18</f>
+        <v>0</v>
+      </c>
+      <c r="L18" s="15">
+        <f>Tabelle1!L18/Tabelle1!$O18</f>
+        <v>0</v>
+      </c>
+      <c r="M18" s="15">
+        <f>Tabelle1!M18/Tabelle1!$O18</f>
+        <v>0</v>
+      </c>
+      <c r="N18" s="15">
+        <f>Tabelle1!N18/Tabelle1!$O18</f>
+        <v>7.7357088877368946E-2</v>
+      </c>
+      <c r="O18" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A19" t="s">
+        <v>165</v>
+      </c>
+      <c r="B19" t="s">
+        <v>166</v>
+      </c>
+      <c r="C19" t="s">
+        <v>125</v>
+      </c>
+      <c r="D19" t="s">
+        <v>75</v>
+      </c>
+      <c r="E19" t="s">
+        <v>263</v>
+      </c>
+      <c r="F19" s="15">
+        <f>Tabelle1!F19/Tabelle1!$O19</f>
+        <v>0.19771126485454329</v>
+      </c>
+      <c r="G19" s="15">
+        <f>Tabelle1!G19/Tabelle1!$O19</f>
+        <v>0</v>
+      </c>
+      <c r="H19" s="15">
+        <f>Tabelle1!H19/Tabelle1!$O19</f>
+        <v>0.30361508334270104</v>
+      </c>
+      <c r="I19" s="15">
+        <f>Tabelle1!I19/Tabelle1!$O19</f>
+        <v>7.577920183950336E-2</v>
+      </c>
+      <c r="J19" s="15">
+        <f>Tabelle1!J19/Tabelle1!$O19</f>
+        <v>8.1587821085437051E-2</v>
+      </c>
+      <c r="K19" s="15">
+        <f>Tabelle1!K19/Tabelle1!$O19</f>
+        <v>0</v>
+      </c>
+      <c r="L19" s="15">
+        <f>Tabelle1!L19/Tabelle1!$O19</f>
+        <v>0</v>
+      </c>
+      <c r="M19" s="15">
+        <f>Tabelle1!M19/Tabelle1!$O19</f>
+        <v>0</v>
+      </c>
+      <c r="N19" s="15">
+        <f>Tabelle1!N19/Tabelle1!$O19</f>
+        <v>0.34130662887781521</v>
+      </c>
+      <c r="O19" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A20" t="s">
+        <v>181</v>
+      </c>
+      <c r="B20" t="s">
+        <v>182</v>
+      </c>
+      <c r="C20" t="s">
+        <v>182</v>
+      </c>
+      <c r="D20" t="s">
+        <v>105</v>
+      </c>
+      <c r="E20" t="s">
+        <v>267</v>
+      </c>
+      <c r="F20" s="15">
+        <f>Tabelle1!F20/Tabelle1!$O20</f>
+        <v>3.5092307323975072E-2</v>
+      </c>
+      <c r="G20" s="15">
+        <f>Tabelle1!G20/Tabelle1!$O20</f>
+        <v>0</v>
+      </c>
+      <c r="H20" s="15">
+        <f>Tabelle1!H20/Tabelle1!$O20</f>
+        <v>0.10022392214995579</v>
+      </c>
+      <c r="I20" s="15">
+        <f>Tabelle1!I20/Tabelle1!$O20</f>
+        <v>0.16107274109377107</v>
+      </c>
+      <c r="J20" s="15">
+        <f>Tabelle1!J20/Tabelle1!$O20</f>
+        <v>0.32380331653725736</v>
+      </c>
+      <c r="K20" s="15">
+        <f>Tabelle1!K20/Tabelle1!$O20</f>
+        <v>0</v>
+      </c>
+      <c r="L20" s="15">
+        <f>Tabelle1!L20/Tabelle1!$O20</f>
+        <v>0</v>
+      </c>
+      <c r="M20" s="15">
+        <f>Tabelle1!M20/Tabelle1!$O20</f>
+        <v>0</v>
+      </c>
+      <c r="N20" s="15">
+        <f>Tabelle1!N20/Tabelle1!$O20</f>
+        <v>0.37980771289504067</v>
+      </c>
+      <c r="O20" s="13">
+        <f t="shared" si="0"/>
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A21" t="s">
+        <v>188</v>
+      </c>
+      <c r="B21" t="s">
+        <v>189</v>
+      </c>
+      <c r="C21" t="s">
+        <v>189</v>
+      </c>
+      <c r="D21" t="s">
+        <v>105</v>
+      </c>
+      <c r="E21" t="s">
+        <v>268</v>
+      </c>
+      <c r="F21" s="15">
+        <f>Tabelle1!F21/Tabelle1!$O21</f>
+        <v>0.13335753761651439</v>
+      </c>
+      <c r="G21" s="15">
+        <f>Tabelle1!G21/Tabelle1!$O21</f>
+        <v>0</v>
+      </c>
+      <c r="H21" s="15">
+        <f>Tabelle1!H21/Tabelle1!$O21</f>
+        <v>7.4158283437427697E-3</v>
+      </c>
+      <c r="I21" s="15">
+        <f>Tabelle1!I21/Tabelle1!$O21</f>
+        <v>0</v>
+      </c>
+      <c r="J21" s="15">
+        <f>Tabelle1!J21/Tabelle1!$O21</f>
+        <v>0</v>
+      </c>
+      <c r="K21" s="15">
+        <f>Tabelle1!K21/Tabelle1!$O21</f>
+        <v>0</v>
+      </c>
+      <c r="L21" s="15">
+        <f>Tabelle1!L21/Tabelle1!$O21</f>
+        <v>0</v>
+      </c>
+      <c r="M21" s="15">
+        <f>Tabelle1!M21/Tabelle1!$O21</f>
+        <v>0.85922663403974275</v>
+      </c>
+      <c r="N21" s="15">
+        <f>Tabelle1!N21/Tabelle1!$O21</f>
+        <v>0</v>
+      </c>
+      <c r="O21" s="13">
+        <f t="shared" si="0"/>
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A22" t="s">
+        <v>195</v>
+      </c>
+      <c r="B22" t="s">
+        <v>196</v>
+      </c>
+      <c r="C22" t="s">
+        <v>197</v>
+      </c>
+      <c r="D22" t="s">
+        <v>105</v>
+      </c>
+      <c r="E22" t="s">
+        <v>269</v>
+      </c>
+      <c r="F22" s="15">
+        <f>Tabelle1!F22/Tabelle1!$O22</f>
+        <v>0.25627313642934685</v>
+      </c>
+      <c r="G22" s="15">
+        <f>Tabelle1!G22/Tabelle1!$O22</f>
+        <v>0</v>
+      </c>
+      <c r="H22" s="15">
+        <f>Tabelle1!H22/Tabelle1!$O22</f>
+        <v>0</v>
+      </c>
+      <c r="I22" s="15">
+        <f>Tabelle1!I22/Tabelle1!$O22</f>
+        <v>0</v>
+      </c>
+      <c r="J22" s="15">
+        <f>Tabelle1!J22/Tabelle1!$O22</f>
+        <v>0.7437268635706531</v>
+      </c>
+      <c r="K22" s="15">
+        <f>Tabelle1!K22/Tabelle1!$O22</f>
+        <v>0</v>
+      </c>
+      <c r="L22" s="15">
+        <f>Tabelle1!L22/Tabelle1!$O22</f>
+        <v>0</v>
+      </c>
+      <c r="M22" s="15">
+        <f>Tabelle1!M22/Tabelle1!$O22</f>
+        <v>0</v>
+      </c>
+      <c r="N22" s="15">
+        <f>Tabelle1!N22/Tabelle1!$O22</f>
+        <v>0</v>
+      </c>
+      <c r="O22" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A23" t="s">
+        <v>198</v>
+      </c>
+      <c r="B23" t="s">
+        <v>199</v>
+      </c>
+      <c r="C23" t="s">
+        <v>200</v>
+      </c>
+      <c r="D23" t="s">
+        <v>201</v>
+      </c>
+      <c r="E23" t="s">
+        <v>270</v>
+      </c>
+      <c r="F23" s="15">
+        <f>Tabelle1!F23/Tabelle1!$O23</f>
+        <v>0.37493741366863303</v>
+      </c>
+      <c r="G23" s="15">
+        <f>Tabelle1!G23/Tabelle1!$O23</f>
+        <v>0</v>
+      </c>
+      <c r="H23" s="15">
+        <f>Tabelle1!H23/Tabelle1!$O23</f>
+        <v>0.33713044517323348</v>
+      </c>
+      <c r="I23" s="15">
+        <f>Tabelle1!I23/Tabelle1!$O23</f>
+        <v>0.17314304401086678</v>
+      </c>
+      <c r="J23" s="15">
+        <f>Tabelle1!J23/Tabelle1!$O23</f>
+        <v>0.11478909714726684</v>
+      </c>
+      <c r="K23" s="15">
+        <f>Tabelle1!K23/Tabelle1!$O23</f>
+        <v>0</v>
+      </c>
+      <c r="L23" s="15">
+        <f>Tabelle1!L23/Tabelle1!$O23</f>
+        <v>0</v>
+      </c>
+      <c r="M23" s="15">
+        <f>Tabelle1!M23/Tabelle1!$O23</f>
+        <v>0</v>
+      </c>
+      <c r="N23" s="15">
+        <f>Tabelle1!N23/Tabelle1!$O23</f>
+        <v>0</v>
+      </c>
+      <c r="O23" s="13">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A24" t="s">
+        <v>206</v>
+      </c>
+      <c r="B24" t="s">
+        <v>207</v>
+      </c>
+      <c r="C24" t="s">
+        <v>192</v>
+      </c>
+      <c r="D24" t="s">
+        <v>201</v>
+      </c>
+      <c r="E24" t="s">
+        <v>261</v>
+      </c>
+      <c r="F24" s="15">
+        <f>Tabelle1!F24/Tabelle1!$O24</f>
+        <v>0.14927160603491776</v>
+      </c>
+      <c r="G24" s="15">
+        <f>Tabelle1!G24/Tabelle1!$O24</f>
+        <v>0</v>
+      </c>
+      <c r="H24" s="15">
+        <f>Tabelle1!H24/Tabelle1!$O24</f>
+        <v>0.74368229504730865</v>
+      </c>
+      <c r="I24" s="15">
+        <f>Tabelle1!I24/Tabelle1!$O24</f>
+        <v>0.10665641166133434</v>
+      </c>
+      <c r="J24" s="15">
+        <f>Tabelle1!J24/Tabelle1!$O24</f>
+        <v>3.8968725643924912E-4</v>
+      </c>
+      <c r="K24" s="15">
+        <f>Tabelle1!K24/Tabelle1!$O24</f>
+        <v>0</v>
+      </c>
+      <c r="L24" s="15">
+        <f>Tabelle1!L24/Tabelle1!$O24</f>
+        <v>0</v>
+      </c>
+      <c r="M24" s="15">
+        <f>Tabelle1!M24/Tabelle1!$O24</f>
+        <v>0</v>
+      </c>
+      <c r="N24" s="15">
+        <f>Tabelle1!N24/Tabelle1!$O24</f>
+        <v>0</v>
+      </c>
+      <c r="O24" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A25" t="s">
+        <v>208</v>
+      </c>
+      <c r="B25" t="s">
+        <v>209</v>
+      </c>
+      <c r="C25" t="s">
+        <v>192</v>
+      </c>
+      <c r="D25" t="s">
+        <v>201</v>
+      </c>
+      <c r="E25" t="s">
+        <v>260</v>
+      </c>
+      <c r="F25" s="15">
+        <f>Tabelle1!F25/Tabelle1!$O25</f>
+        <v>0.10325131641773541</v>
+      </c>
+      <c r="G25" s="15">
+        <f>Tabelle1!G25/Tabelle1!$O25</f>
+        <v>0</v>
+      </c>
+      <c r="H25" s="15">
+        <f>Tabelle1!H25/Tabelle1!$O25</f>
+        <v>0.65355640134574999</v>
+      </c>
+      <c r="I25" s="15">
+        <f>Tabelle1!I25/Tabelle1!$O25</f>
+        <v>5.694895792434277E-2</v>
+      </c>
+      <c r="J25" s="15">
+        <f>Tabelle1!J25/Tabelle1!$O25</f>
+        <v>9.849864142894172E-4</v>
+      </c>
+      <c r="K25" s="15">
+        <f>Tabelle1!K25/Tabelle1!$O25</f>
+        <v>3.5389714781289126E-2</v>
+      </c>
+      <c r="L25" s="15">
+        <f>Tabelle1!L25/Tabelle1!$O25</f>
+        <v>0</v>
+      </c>
+      <c r="M25" s="15">
+        <f>Tabelle1!M25/Tabelle1!$O25</f>
+        <v>0</v>
+      </c>
+      <c r="N25" s="15">
+        <f>Tabelle1!N25/Tabelle1!$O25</f>
+        <v>0.14986862311659319</v>
+      </c>
+      <c r="O25" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A26" t="s">
+        <v>211</v>
+      </c>
+      <c r="B26" t="s">
+        <v>212</v>
+      </c>
+      <c r="C26" t="s">
+        <v>213</v>
+      </c>
+      <c r="D26" t="s">
+        <v>214</v>
+      </c>
+      <c r="E26" t="s">
+        <v>259</v>
+      </c>
+      <c r="F26" s="15">
+        <f>Tabelle1!F26/Tabelle1!$O26</f>
+        <v>0.31230169308824107</v>
+      </c>
+      <c r="G26" s="15">
+        <f>Tabelle1!G26/Tabelle1!$O26</f>
+        <v>0</v>
+      </c>
+      <c r="H26" s="15">
+        <f>Tabelle1!H26/Tabelle1!$O26</f>
+        <v>0.66099764107940606</v>
+      </c>
+      <c r="I26" s="15">
+        <f>Tabelle1!I26/Tabelle1!$O26</f>
+        <v>2.6700665832352768E-2</v>
+      </c>
+      <c r="J26" s="15">
+        <f>Tabelle1!J26/Tabelle1!$O26</f>
+        <v>0</v>
+      </c>
+      <c r="K26" s="15">
+        <f>Tabelle1!K26/Tabelle1!$O26</f>
+        <v>0</v>
+      </c>
+      <c r="L26" s="15">
+        <f>Tabelle1!L26/Tabelle1!$O26</f>
+        <v>0</v>
+      </c>
+      <c r="M26" s="15">
+        <f>Tabelle1!M26/Tabelle1!$O26</f>
+        <v>0</v>
+      </c>
+      <c r="N26" s="15">
+        <f>Tabelle1!N26/Tabelle1!$O26</f>
+        <v>0</v>
+      </c>
+      <c r="O26" s="13">
+        <f t="shared" si="0"/>
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A27" t="s">
+        <v>215</v>
+      </c>
+      <c r="B27" t="s">
+        <v>271</v>
+      </c>
+      <c r="C27" t="s">
+        <v>271</v>
+      </c>
+      <c r="D27" t="s">
+        <v>214</v>
+      </c>
+      <c r="E27" t="s">
+        <v>271</v>
+      </c>
+      <c r="F27" s="15">
+        <f>Tabelle1!F27/Tabelle1!$O27</f>
+        <v>0.99474846824537866</v>
+      </c>
+      <c r="G27" s="15">
+        <f>Tabelle1!G27/Tabelle1!$O27</f>
+        <v>0</v>
+      </c>
+      <c r="H27" s="15">
+        <f>Tabelle1!H27/Tabelle1!$O27</f>
+        <v>0</v>
+      </c>
+      <c r="I27" s="15">
+        <f>Tabelle1!I27/Tabelle1!$O27</f>
+        <v>5.2515317546212329E-3</v>
+      </c>
+      <c r="J27" s="15">
+        <f>Tabelle1!J27/Tabelle1!$O27</f>
+        <v>0</v>
+      </c>
+      <c r="K27" s="15">
+        <f>Tabelle1!K27/Tabelle1!$O27</f>
+        <v>0</v>
+      </c>
+      <c r="L27" s="15">
+        <f>Tabelle1!L27/Tabelle1!$O27</f>
+        <v>0</v>
+      </c>
+      <c r="M27" s="15">
+        <f>Tabelle1!M27/Tabelle1!$O27</f>
+        <v>0</v>
+      </c>
+      <c r="N27" s="15">
+        <f>Tabelle1!N27/Tabelle1!$O27</f>
+        <v>0</v>
+      </c>
+      <c r="O27" s="13">
+        <f t="shared" si="0"/>
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A28" t="s">
+        <v>217</v>
+      </c>
+      <c r="B28" t="s">
+        <v>218</v>
+      </c>
+      <c r="C28" t="s">
+        <v>219</v>
+      </c>
+      <c r="D28" t="s">
+        <v>214</v>
+      </c>
+      <c r="E28" t="s">
+        <v>258</v>
+      </c>
+      <c r="F28" s="15">
+        <f>Tabelle1!F28/Tabelle1!$O28</f>
+        <v>0.28173036563200293</v>
+      </c>
+      <c r="G28" s="15">
+        <f>Tabelle1!G28/Tabelle1!$O28</f>
+        <v>0.26322674416122654</v>
+      </c>
+      <c r="H28" s="15">
+        <f>Tabelle1!H28/Tabelle1!$O28</f>
+        <v>0.45405180322580252</v>
+      </c>
+      <c r="I28" s="15">
+        <f>Tabelle1!I28/Tabelle1!$O28</f>
+        <v>0</v>
+      </c>
+      <c r="J28" s="15">
+        <f>Tabelle1!J28/Tabelle1!$O28</f>
+        <v>9.9108698096799213E-4</v>
+      </c>
+      <c r="K28" s="15">
+        <f>Tabelle1!K28/Tabelle1!$O28</f>
+        <v>0</v>
+      </c>
+      <c r="L28" s="15">
+        <f>Tabelle1!L28/Tabelle1!$O28</f>
+        <v>0</v>
+      </c>
+      <c r="M28" s="15">
+        <f>Tabelle1!M28/Tabelle1!$O28</f>
+        <v>0</v>
+      </c>
+      <c r="N28" s="15">
+        <f>Tabelle1!N28/Tabelle1!$O28</f>
+        <v>0</v>
+      </c>
+      <c r="O28" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A29" t="s">
+        <v>230</v>
+      </c>
+      <c r="B29" t="s">
+        <v>231</v>
+      </c>
+      <c r="C29" t="s">
+        <v>231</v>
+      </c>
+      <c r="D29" t="s">
+        <v>231</v>
+      </c>
+      <c r="E29" t="s">
+        <v>272</v>
+      </c>
+      <c r="F29" s="15">
+        <f>Tabelle1!F29/Tabelle1!$O29</f>
+        <v>0</v>
+      </c>
+      <c r="G29" s="15">
+        <f>Tabelle1!G29/Tabelle1!$O29</f>
+        <v>0</v>
+      </c>
+      <c r="H29" s="15">
+        <f>Tabelle1!H29/Tabelle1!$O29</f>
+        <v>0.352912804442229</v>
+      </c>
+      <c r="I29" s="15">
+        <f>Tabelle1!I29/Tabelle1!$O29</f>
+        <v>0.34897923757000343</v>
+      </c>
+      <c r="J29" s="15">
+        <f>Tabelle1!J29/Tabelle1!$O29</f>
+        <v>0.15416709603881129</v>
+      </c>
+      <c r="K29" s="15">
+        <f>Tabelle1!K29/Tabelle1!$O29</f>
+        <v>0</v>
+      </c>
+      <c r="L29" s="15">
+        <f>Tabelle1!L29/Tabelle1!$O29</f>
+        <v>0</v>
+      </c>
+      <c r="M29" s="15">
+        <f>Tabelle1!M29/Tabelle1!$O29</f>
+        <v>0</v>
+      </c>
+      <c r="N29" s="15">
+        <f>Tabelle1!N29/Tabelle1!$O29</f>
+        <v>0.14394086194895631</v>
+      </c>
+      <c r="O29" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A30" t="s">
+        <v>232</v>
+      </c>
+      <c r="B30" t="s">
+        <v>233</v>
+      </c>
+      <c r="C30" t="s">
+        <v>233</v>
+      </c>
+      <c r="D30" t="s">
+        <v>234</v>
+      </c>
+      <c r="E30" t="s">
+        <v>272</v>
+      </c>
+      <c r="F30" s="15">
+        <f>Tabelle1!F30/Tabelle1!$O30</f>
+        <v>2.1605732947277793E-2</v>
+      </c>
+      <c r="G30" s="15">
+        <f>Tabelle1!G30/Tabelle1!$O30</f>
+        <v>0</v>
+      </c>
+      <c r="H30" s="15">
+        <f>Tabelle1!H30/Tabelle1!$O30</f>
+        <v>2.0531347343911412E-2</v>
+      </c>
+      <c r="I30" s="15">
+        <f>Tabelle1!I30/Tabelle1!$O30</f>
+        <v>5.2651825227601493E-2</v>
+      </c>
+      <c r="J30" s="15">
+        <f>Tabelle1!J30/Tabelle1!$O30</f>
+        <v>2.7590639020989325E-2</v>
+      </c>
+      <c r="K30" s="15">
+        <f>Tabelle1!K30/Tabelle1!$O30</f>
+        <v>0.73621203544496217</v>
+      </c>
+      <c r="L30" s="15">
+        <f>Tabelle1!L30/Tabelle1!$O30</f>
+        <v>0</v>
+      </c>
+      <c r="M30" s="15">
+        <f>Tabelle1!M30/Tabelle1!$O30</f>
+        <v>0</v>
+      </c>
+      <c r="N30" s="15">
+        <f>Tabelle1!N30/Tabelle1!$O30</f>
+        <v>0.14140842001525783</v>
+      </c>
+      <c r="O30" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A31" t="s">
+        <v>235</v>
+      </c>
+      <c r="B31" t="s">
+        <v>236</v>
+      </c>
+      <c r="C31" t="s">
+        <v>237</v>
+      </c>
+      <c r="D31" t="s">
+        <v>22</v>
+      </c>
+      <c r="E31" t="s">
+        <v>22</v>
+      </c>
+      <c r="F31" s="15">
+        <f>Tabelle1!F31/Tabelle1!$O31</f>
+        <v>1.900452702607873E-2</v>
+      </c>
+      <c r="G31" s="15">
+        <f>Tabelle1!G31/Tabelle1!$O31</f>
+        <v>0</v>
+      </c>
+      <c r="H31" s="15">
+        <f>Tabelle1!H31/Tabelle1!$O31</f>
+        <v>1.5439234500000208E-2</v>
+      </c>
+      <c r="I31" s="15">
+        <f>Tabelle1!I31/Tabelle1!$O31</f>
+        <v>0.37809605856859391</v>
+      </c>
+      <c r="J31" s="15">
+        <f>Tabelle1!J31/Tabelle1!$O31</f>
+        <v>5.5524503240166181E-2</v>
+      </c>
+      <c r="K31" s="15">
+        <f>Tabelle1!K31/Tabelle1!$O31</f>
+        <v>2.2371333123969331E-3</v>
+      </c>
+      <c r="L31" s="15">
+        <f>Tabelle1!L31/Tabelle1!$O31</f>
+        <v>0</v>
+      </c>
+      <c r="M31" s="15">
+        <f>Tabelle1!M31/Tabelle1!$O31</f>
+        <v>0</v>
+      </c>
+      <c r="N31" s="15">
+        <f>Tabelle1!N31/Tabelle1!$O31</f>
+        <v>0.52969854335276401</v>
+      </c>
+      <c r="O31" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A32" t="s">
+        <v>238</v>
+      </c>
+      <c r="B32" t="s">
+        <v>239</v>
+      </c>
+      <c r="C32" t="s">
+        <v>239</v>
+      </c>
+      <c r="D32" t="s">
+        <v>240</v>
+      </c>
+      <c r="E32" t="s">
+        <v>257</v>
+      </c>
+      <c r="F32" s="15">
+        <f>Tabelle1!F32/Tabelle1!$O32</f>
+        <v>3.8241927667276797E-3</v>
+      </c>
+      <c r="G32" s="15">
+        <f>Tabelle1!G32/Tabelle1!$O32</f>
+        <v>0</v>
+      </c>
+      <c r="H32" s="15">
+        <f>Tabelle1!H32/Tabelle1!$O32</f>
+        <v>1.2167570693687615E-2</v>
+      </c>
+      <c r="I32" s="15">
+        <f>Tabelle1!I32/Tabelle1!$O32</f>
+        <v>0.10900146216268282</v>
+      </c>
+      <c r="J32" s="15">
+        <f>Tabelle1!J32/Tabelle1!$O32</f>
+        <v>1.1855395992430956E-2</v>
+      </c>
+      <c r="K32" s="15">
+        <f>Tabelle1!K32/Tabelle1!$O32</f>
+        <v>3.9228931856469647E-2</v>
+      </c>
+      <c r="L32" s="15">
+        <f>Tabelle1!L32/Tabelle1!$O32</f>
+        <v>0.4455365380608578</v>
+      </c>
+      <c r="M32" s="15">
+        <f>Tabelle1!M32/Tabelle1!$O32</f>
+        <v>0</v>
+      </c>
+      <c r="N32" s="15">
+        <f>Tabelle1!N32/Tabelle1!$O32</f>
+        <v>0.37838590846714359</v>
+      </c>
+      <c r="O32" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A33" t="s">
+        <v>241</v>
+      </c>
+      <c r="B33" t="s">
+        <v>243</v>
+      </c>
+      <c r="C33" t="s">
+        <v>242</v>
+      </c>
+      <c r="D33" t="s">
+        <v>243</v>
+      </c>
+      <c r="E33" t="s">
+        <v>23</v>
+      </c>
+      <c r="F33" s="15">
+        <f>Tabelle1!F33/Tabelle1!$O33</f>
+        <v>9.7401202589069327E-2</v>
+      </c>
+      <c r="G33" s="15">
+        <f>Tabelle1!G33/Tabelle1!$O33</f>
+        <v>5.996295090999737E-2</v>
+      </c>
+      <c r="H33" s="15">
+        <f>Tabelle1!H33/Tabelle1!$O33</f>
+        <v>3.5508941457038361E-2</v>
+      </c>
+      <c r="I33" s="15">
+        <f>Tabelle1!I33/Tabelle1!$O33</f>
+        <v>5.5467093617606156E-2</v>
+      </c>
+      <c r="J33" s="15">
+        <f>Tabelle1!J33/Tabelle1!$O33</f>
+        <v>0.52188590855556349</v>
+      </c>
+      <c r="K33" s="15">
+        <f>Tabelle1!K33/Tabelle1!$O33</f>
+        <v>0</v>
+      </c>
+      <c r="L33" s="15">
+        <f>Tabelle1!L33/Tabelle1!$O33</f>
+        <v>0.12787797696720959</v>
+      </c>
+      <c r="M33" s="15">
+        <f>Tabelle1!M33/Tabelle1!$O33</f>
+        <v>3.7222020221106399E-2</v>
+      </c>
+      <c r="N33" s="15">
+        <f>Tabelle1!N33/Tabelle1!$O33</f>
+        <v>6.4673905682409313E-2</v>
+      </c>
+      <c r="O33" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>